<commit_message>
New helper class and diffrentlogic for assignment test added
</commit_message>
<xml_diff>
--- a/MYFramework/src/main/java/helper/exceldata/LMS_TestData.xlsx
+++ b/MYFramework/src/main/java/helper/exceldata/LMS_TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parag.borawake\git\NewFrameworks_1\MYFramework\src\main\java\helper\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2940ADE9-5690-4F31-A6B5-BE7D9E3962D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005DFE5C-954A-45DD-84AE-3ED0D57B4F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{88A90910-4565-483B-8D0E-2283B58769B8}"/>
   </bookViews>
   <sheets>
     <sheet name="LMSData" sheetId="1" r:id="rId1"/>
+    <sheet name="Domain" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Libraries</t>
   </si>
   <si>
-    <t>COM_TEST;COM_TEST1</t>
-  </si>
-  <si>
     <t>Country/Region;City</t>
   </si>
   <si>
@@ -104,9 +102,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>TestGroup1</t>
-  </si>
-  <si>
     <t>TestGroup2</t>
   </si>
   <si>
@@ -116,23 +111,44 @@
     <t>Group1 Value</t>
   </si>
   <si>
-    <t>Test8901</t>
-  </si>
-  <si>
-    <t>Test0982</t>
-  </si>
-  <si>
-    <t>Test8093</t>
-  </si>
-  <si>
-    <t>Core test A ; Core test B</t>
+    <t>CORE TEST A;CORE TEST B</t>
+  </si>
+  <si>
+    <t>Gamification_Catalog;COM_TEST</t>
+  </si>
+  <si>
+    <t>CORE TEST B</t>
+  </si>
+  <si>
+    <t>CORE TEST A</t>
+  </si>
+  <si>
+    <t>EXTERNAL</t>
+  </si>
+  <si>
+    <t>Names</t>
+  </si>
+  <si>
+    <t>CORE TEST A;CORE TEST B;External</t>
+  </si>
+  <si>
+    <t>20200722;GENERAL</t>
+  </si>
+  <si>
+    <t>CORE TEST A;EXTERNAL</t>
+  </si>
+  <si>
+    <t>COM_TEST;TestLirbrary</t>
+  </si>
+  <si>
+    <t>TestGroup1;TestGroup2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,8 +156,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +173,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -182,12 +210,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A23C6E4B-9866-4E64-B330-64A5CE466473}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -515,172 +544,220 @@
     <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.81640625" customWidth="1"/>
     <col min="7" max="8" width="20.7265625" customWidth="1"/>
-    <col min="9" max="9" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.08984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.7265625" customWidth="1"/>
     <col min="18" max="18" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
       <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>18</v>
+      <c r="S1" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
+      <c r="S2" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C3" s="2" t="s">
-        <v>28</v>
-      </c>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="M3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
+      <c r="S3" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C4" s="2" t="s">
-        <v>29</v>
-      </c>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="M4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63030FF-6010-44ED-B4BA-5A1F3CF5BD87}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes in assignment profile and excel
</commit_message>
<xml_diff>
--- a/MYFramework/src/main/java/helper/exceldata/LMS_TestData.xlsx
+++ b/MYFramework/src/main/java/helper/exceldata/LMS_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parag.borawake\git\NewFrameworks_1\MYFramework\src\main\java\helper\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005DFE5C-954A-45DD-84AE-3ED0D57B4F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A022750A-9986-4FEF-87CE-EAF1E60E73E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{88A90910-4565-483B-8D0E-2283B58769B8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Libraries</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>TestGroup1;TestGroup2</t>
+  </si>
+  <si>
+    <t>CORE TEST A;CORE TEST E</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -663,7 +666,7 @@
         <v>32</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
New pages and CreateNewLibraries
</commit_message>
<xml_diff>
--- a/MYFramework/src/main/java/helper/exceldata/LMS_TestData.xlsx
+++ b/MYFramework/src/main/java/helper/exceldata/LMS_TestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parag.borawake\git\NewFrameworks_1\MYFramework\src\main\java\helper\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30913EA6-0347-48B0-A9C0-F9076937C716}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0090A297-2AB1-4379-A8E8-11BEEE3DAC69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{88A90910-4565-483B-8D0E-2283B58769B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{88A90910-4565-483B-8D0E-2283B58769B8}"/>
   </bookViews>
   <sheets>
     <sheet name="LMSData" sheetId="1" r:id="rId1"/>
-    <sheet name="Domain" sheetId="2" r:id="rId2"/>
+    <sheet name="AddLibraries" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Libraries</t>
   </si>
@@ -60,9 +60,6 @@
     <t>bparag</t>
   </si>
   <si>
-    <t>borawake81</t>
-  </si>
-  <si>
     <t>Create Group1</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>CORE TEST B</t>
   </si>
   <si>
-    <t>CORE TEST A</t>
-  </si>
-  <si>
     <t>EXTERNAL</t>
   </si>
   <si>
@@ -151,6 +145,33 @@
   </si>
   <si>
     <t>Group2Attribute</t>
+  </si>
+  <si>
+    <t>Discount Rate</t>
+  </si>
+  <si>
+    <t>Contact's Email</t>
+  </si>
+  <si>
+    <t>Add Curriculum</t>
+  </si>
+  <si>
+    <t>Test Library</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200717;20200720 </t>
+  </si>
+  <si>
+    <t>LibraryID</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>welcome123</t>
+  </si>
+  <si>
+    <t>username</t>
   </si>
 </sst>
 </file>
@@ -172,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +203,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,12 +246,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -542,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A23C6E4B-9866-4E64-B330-64A5CE466473}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,14 +595,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -582,13 +611,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>0</v>
@@ -597,45 +626,45 @@
         <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -644,13 +673,13 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>1</v>
@@ -659,23 +688,25 @@
         <v>1</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -683,23 +714,23 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="2"/>
@@ -707,10 +738,12 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -718,23 +751,23 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="2"/>
@@ -742,7 +775,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -753,37 +786,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63030FF-6010-44ED-B4BA-5A1F3CF5BD87}">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D288D5AE-1DEC-4915-8764-FA569969EA82}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>45</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>28</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New pages for catlouge and changes in "AssignmentProfileTest" page is completed
</commit_message>
<xml_diff>
--- a/MYFramework/src/main/java/helper/exceldata/LMS_TestData.xlsx
+++ b/MYFramework/src/main/java/helper/exceldata/LMS_TestData.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parag.borawake\git\NewFrameworks_1\MYFramework\src\main\java\helper\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0090A297-2AB1-4379-A8E8-11BEEE3DAC69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{913481C4-9D2D-4CB5-A088-28F7DA3C6FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{88A90910-4565-483B-8D0E-2283B58769B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{88A90910-4565-483B-8D0E-2283B58769B8}"/>
   </bookViews>
   <sheets>
     <sheet name="LMSData" sheetId="1" r:id="rId1"/>
     <sheet name="AddLibraries" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -246,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -254,7 +255,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A23C6E4B-9866-4E64-B330-64A5CE466473}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D288D5AE-1DEC-4915-8764-FA569969EA82}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -824,7 +824,7 @@
       <c r="G1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
screenshots and mousehover class
</commit_message>
<xml_diff>
--- a/MYFramework/src/main/java/helper/exceldata/LMS_TestData.xlsx
+++ b/MYFramework/src/main/java/helper/exceldata/LMS_TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parag.borawake\git\NewFrameworks_1\MYFramework\src\main\java\helper\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EAE843-AD21-4A92-B3D4-73CE6D44DB70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47241B00-2BFF-47B9-8517-1010D6A4A65F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{88A90910-4565-483B-8D0E-2283B58769B8}"/>
   </bookViews>
   <sheets>
     <sheet name="LMSData" sheetId="1" r:id="rId1"/>
-    <sheet name="SecurityDomain" sheetId="2" r:id="rId2"/>
+    <sheet name="ActionTest" sheetId="3" r:id="rId2"/>
+    <sheet name="SecurityDomain" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Libraries</t>
   </si>
@@ -166,13 +167,22 @@
   </si>
   <si>
     <t>welcome234</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>borawake81</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +196,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +221,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -234,13 +258,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,6 +781,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CD6CA3-228F-45D8-B840-B5561D888412}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>9850049989</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63030FF-6010-44ED-B4BA-5A1F3CF5BD87}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A10"/>

</xml_diff>